<commit_message>
20250702 Merge file upgrade
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202506/Review 202506/Coen/ECHP_Composition_20250618_132119.xlsx
+++ b/GUI + Reviews/202506/Review 202506/Coen/ECHP_Composition_20250618_132119.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202506/Review 202506/Coen/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_16D17222F64D0103732C4C8C3D57166C5CE6B18A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90EB3141-7F33-40CA-90F4-4C1E08061328}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ECHP Composition" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="62">
   <si>
     <t>Company</t>
   </si>
@@ -194,13 +200,19 @@
   </si>
   <si>
     <t>CHF</t>
+  </si>
+  <si>
+    <t>AMRIZE</t>
+  </si>
+  <si>
+    <t>CH1430134226</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -263,13 +275,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -307,7 +327,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -341,6 +361,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -375,9 +396,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -550,14 +572,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:H4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -583,7 +607,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -609,7 +633,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -635,18 +659,18 @@
         <v>59</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
         <v>57</v>
       </c>
       <c r="D4">
-        <v>1004326</v>
+        <v>579124630</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -654,586 +678,615 @@
       <c r="F4">
         <v>1</v>
       </c>
-      <c r="G4" t="s">
-        <v>58</v>
+      <c r="G4">
+        <v>45831</v>
       </c>
       <c r="H4" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
       <c r="B5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5">
+        <v>1004326</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>58</v>
+      </c>
+      <c r="H5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
         <v>35</v>
       </c>
-      <c r="C5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D5">
+      <c r="C6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D6">
         <v>134099</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>0.85</v>
       </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>58</v>
-      </c>
-      <c r="H5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8">
-      <c r="A6" t="s">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>36</v>
       </c>
-      <c r="C6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D6">
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7">
         <v>537582100</v>
       </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>58</v>
-      </c>
-      <c r="H6" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8">
-      <c r="A7" t="s">
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>58</v>
+      </c>
+      <c r="H7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>37</v>
       </c>
-      <c r="C7" t="s">
-        <v>57</v>
-      </c>
-      <c r="D7">
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+      <c r="D8">
         <v>237897630</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>0.5</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-      <c r="G7" t="s">
-        <v>58</v>
-      </c>
-      <c r="H7" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8">
-      <c r="A8" t="s">
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>13</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B9" t="s">
         <v>38</v>
       </c>
-      <c r="C8" t="s">
-        <v>57</v>
-      </c>
-      <c r="D8">
+      <c r="C9" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9">
         <v>33922405</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>0.95</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-      <c r="G8" t="s">
-        <v>58</v>
-      </c>
-      <c r="H8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8">
-      <c r="A9" t="s">
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>39</v>
       </c>
-      <c r="C9" t="s">
-        <v>57</v>
-      </c>
-      <c r="D9">
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10">
         <v>9233586</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>0.9</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>58</v>
-      </c>
-      <c r="H9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8">
-      <c r="A10" t="s">
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+      <c r="H10" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>40</v>
       </c>
-      <c r="C10" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10">
+      <c r="C11" t="s">
+        <v>57</v>
+      </c>
+      <c r="D11">
         <v>579124630</v>
       </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-      <c r="G10" t="s">
-        <v>58</v>
-      </c>
-      <c r="H10" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8">
-      <c r="A11" t="s">
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>58</v>
+      </c>
+      <c r="H11" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>41</v>
       </c>
-      <c r="C11" t="s">
-        <v>57</v>
-      </c>
-      <c r="D11">
+      <c r="C12" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12">
         <v>72226180</v>
       </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-      <c r="G11" t="s">
-        <v>58</v>
-      </c>
-      <c r="H11" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8">
-      <c r="A12" t="s">
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B13" t="s">
         <v>42</v>
       </c>
-      <c r="C12" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12">
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13">
         <v>2576520000</v>
       </c>
-      <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-      <c r="G12" t="s">
-        <v>58</v>
-      </c>
-      <c r="H12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8">
-      <c r="A13" t="s">
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>58</v>
+      </c>
+      <c r="H13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B14" t="s">
         <v>43</v>
       </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13">
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14">
         <v>2112421900</v>
       </c>
-      <c r="E13">
+      <c r="E14">
         <v>0.95</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-      <c r="G13" t="s">
-        <v>58</v>
-      </c>
-      <c r="H13" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8">
-      <c r="A14" t="s">
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>58</v>
+      </c>
+      <c r="H14" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>44</v>
       </c>
-      <c r="C14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14">
+      <c r="C15" t="s">
+        <v>57</v>
+      </c>
+      <c r="D15">
         <v>26700000</v>
       </c>
-      <c r="E14">
+      <c r="E15">
         <v>0.85</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-      <c r="G14" t="s">
-        <v>58</v>
-      </c>
-      <c r="H14" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8">
-      <c r="A15" t="s">
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>58</v>
+      </c>
+      <c r="H15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B16" t="s">
         <v>45</v>
       </c>
-      <c r="C15" t="s">
-        <v>57</v>
-      </c>
-      <c r="D15">
+      <c r="C16" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16">
         <v>702562700</v>
       </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>58</v>
-      </c>
-      <c r="H15" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8">
-      <c r="A16" t="s">
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16" t="s">
+        <v>58</v>
+      </c>
+      <c r="H16" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B17" t="s">
         <v>46</v>
       </c>
-      <c r="C16" t="s">
-        <v>57</v>
-      </c>
-      <c r="D16">
+      <c r="C17" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17">
         <v>440000000</v>
       </c>
-      <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" t="s">
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>58</v>
+      </c>
+      <c r="H17" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B18" t="s">
         <v>47</v>
       </c>
-      <c r="C17" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17">
+      <c r="C18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D18">
         <v>40716830</v>
       </c>
-      <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>58</v>
-      </c>
-      <c r="H17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18" t="s">
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18">
+      <c r="C19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D19">
         <v>194777280</v>
       </c>
-      <c r="E18">
+      <c r="E19">
         <v>0.8</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-      <c r="G18" t="s">
-        <v>58</v>
-      </c>
-      <c r="H18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19" t="s">
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19" t="s">
+        <v>58</v>
+      </c>
+      <c r="H19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>49</v>
       </c>
-      <c r="C19" t="s">
-        <v>57</v>
-      </c>
-      <c r="D19">
+      <c r="C20" t="s">
+        <v>57</v>
+      </c>
+      <c r="D20">
         <v>160479300</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-      <c r="G19" t="s">
-        <v>58</v>
-      </c>
-      <c r="H19" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" t="s">
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="C20" t="s">
-        <v>57</v>
-      </c>
-      <c r="D20">
+      <c r="C21" t="s">
+        <v>57</v>
+      </c>
+      <c r="D21">
         <v>59626810</v>
       </c>
-      <c r="E20">
+      <c r="E21">
         <v>0.85</v>
       </c>
-      <c r="F20">
-        <v>1</v>
-      </c>
-      <c r="G20" t="s">
-        <v>58</v>
-      </c>
-      <c r="H20" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21" t="s">
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21" t="s">
+        <v>58</v>
+      </c>
+      <c r="H21" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>51</v>
       </c>
-      <c r="C21" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21">
+      <c r="C22" t="s">
+        <v>57</v>
+      </c>
+      <c r="D22">
         <v>159455250</v>
       </c>
-      <c r="E21">
+      <c r="E22">
         <v>0.75</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-      <c r="G21" t="s">
-        <v>58</v>
-      </c>
-      <c r="H21" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22" t="s">
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H22" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>27</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
         <v>52</v>
       </c>
-      <c r="C22" t="s">
-        <v>57</v>
-      </c>
-      <c r="D22">
+      <c r="C23" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23">
         <v>28727518</v>
       </c>
-      <c r="E22">
-        <v>1</v>
-      </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-      <c r="G22" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8">
-      <c r="A23" t="s">
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23" t="s">
+        <v>58</v>
+      </c>
+      <c r="H23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>28</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>53</v>
       </c>
-      <c r="C23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23">
+      <c r="C24" t="s">
+        <v>57</v>
+      </c>
+      <c r="D24">
         <v>317497300</v>
       </c>
-      <c r="E23">
+      <c r="E24">
         <v>0.9</v>
       </c>
-      <c r="F23">
-        <v>1</v>
-      </c>
-      <c r="G23" t="s">
-        <v>58</v>
-      </c>
-      <c r="H23" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8">
-      <c r="A24" t="s">
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24" t="s">
+        <v>58</v>
+      </c>
+      <c r="H24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>29</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>54</v>
       </c>
-      <c r="C24" t="s">
-        <v>57</v>
-      </c>
-      <c r="D24">
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25">
         <v>51801945</v>
       </c>
-      <c r="E24">
+      <c r="E25">
         <v>0.5</v>
       </c>
-      <c r="F24">
-        <v>1</v>
-      </c>
-      <c r="G24" t="s">
-        <v>58</v>
-      </c>
-      <c r="H24" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8">
-      <c r="A25" t="s">
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25" t="s">
+        <v>58</v>
+      </c>
+      <c r="H25" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>30</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B26" t="s">
         <v>55</v>
       </c>
-      <c r="C25" t="s">
-        <v>57</v>
-      </c>
-      <c r="D25">
+      <c r="C26" t="s">
+        <v>57</v>
+      </c>
+      <c r="D26">
         <v>3341581800</v>
       </c>
-      <c r="E25">
+      <c r="E26">
         <v>0.9</v>
       </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8">
-      <c r="A26" t="s">
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>58</v>
+      </c>
+      <c r="H26" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>31</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>56</v>
       </c>
-      <c r="C26" t="s">
-        <v>57</v>
-      </c>
-      <c r="D26">
+      <c r="C27" t="s">
+        <v>57</v>
+      </c>
+      <c r="D27">
         <v>146355760</v>
       </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-      <c r="G26" t="s">
-        <v>58</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>58</v>
+      </c>
+      <c r="H27" t="s">
         <v>59</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter>
+    <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFFEF00 PRIVATE</oddFooter>
+  </headerFooter>
 </worksheet>
 </file>
</xml_diff>